<commit_message>
chore: :wrench: minor edits
</commit_message>
<xml_diff>
--- a/reports/metrics/metrics.xlsx
+++ b/reports/metrics/metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jensen/Desktop/recommendation-systems/reports/metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625C387B-88A1-6F45-ACC4-88D0F641449D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF173EC-D4B3-2145-BA6F-99BC76C22E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{1BBCF0FA-60AB-C24D-8479-9EF9DCCACDF3}"/>
+    <workbookView xWindow="28620" yWindow="7480" windowWidth="14400" windowHeight="17500" xr2:uid="{1BBCF0FA-60AB-C24D-8479-9EF9DCCACDF3}"/>
   </bookViews>
   <sheets>
     <sheet name="metrics" sheetId="1" r:id="rId1"/>
@@ -126,10 +126,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -449,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537E13BF-5D9A-5A41-BC93-BEA38BAFFAF2}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,10 +485,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="2">
-        <v>1.485E-2</v>
+        <v>1.4930000000000001E-2</v>
       </c>
       <c r="E2" s="2">
-        <v>0.88492999999999999</v>
+        <v>0.88488</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -503,10 +502,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>2.1739999999999999E-2</v>
+        <v>2.2280000000000001E-2</v>
       </c>
       <c r="E3" s="2">
-        <v>0.90641000000000005</v>
+        <v>0.90627999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -520,10 +519,10 @@
         <v>15</v>
       </c>
       <c r="D4" s="2">
-        <v>2.64E-2</v>
+        <v>2.664E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>0.92096999999999996</v>
+        <v>0.92090000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -537,10 +536,10 @@
         <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>3.0530000000000002E-2</v>
+        <v>3.0949999999999998E-2</v>
       </c>
       <c r="E5" s="2">
-        <v>0.93147000000000002</v>
+        <v>0.93125999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -553,10 +552,10 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>8.6700000000000006E-3</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0.83228999999999997</v>
       </c>
     </row>
@@ -570,10 +569,10 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>1.355E-2</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0.85758000000000001</v>
       </c>
     </row>
@@ -587,10 +586,10 @@
       <c r="C8">
         <v>15</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>1.7080000000000001E-2</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.86792000000000002</v>
       </c>
     </row>
@@ -604,10 +603,10 @@
       <c r="C9">
         <v>20</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>2.0889999999999999E-2</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0.87419999999999998</v>
       </c>
     </row>
@@ -621,10 +620,10 @@
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>7.62E-3</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.88465000000000005</v>
       </c>
     </row>
@@ -638,10 +637,10 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>1.0749999999999999E-2</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>0.90600000000000003</v>
       </c>
     </row>
@@ -655,10 +654,10 @@
       <c r="C12">
         <v>15</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>1.38E-2</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>0.91437000000000002</v>
       </c>
     </row>
@@ -672,10 +671,10 @@
       <c r="C13">
         <v>20</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>1.6209999999999999E-2</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>0.92122999999999999</v>
       </c>
     </row>
@@ -689,10 +688,10 @@
       <c r="C14">
         <v>5</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>1.9000000000000001E-4</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>0.96479000000000004</v>
       </c>
     </row>
@@ -706,10 +705,10 @@
       <c r="C15">
         <v>10</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>4.6000000000000001E-4</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>0.95774999999999999</v>
       </c>
     </row>
@@ -723,10 +722,10 @@
       <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>9.6000000000000002E-4</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>0.95604999999999996</v>
       </c>
     </row>
@@ -740,10 +739,10 @@
       <c r="C17">
         <v>20</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>1.2800000000000001E-3</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>0.95740000000000003</v>
       </c>
     </row>
@@ -757,10 +756,10 @@
       <c r="C18">
         <v>5</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>1.3610000000000001E-2</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <v>0.93771000000000004</v>
       </c>
     </row>
@@ -774,10 +773,10 @@
       <c r="C19">
         <v>10</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <v>2.1770000000000001E-2</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <v>0.94206999999999996</v>
       </c>
     </row>
@@ -791,10 +790,10 @@
       <c r="C20">
         <v>15</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <v>2.9270000000000001E-2</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <v>0.94574000000000003</v>
       </c>
     </row>
@@ -808,10 +807,10 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <v>3.5839999999999997E-2</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <v>0.94881000000000004</v>
       </c>
     </row>
@@ -825,10 +824,10 @@
       <c r="C22">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <v>2.4199999999999998E-3</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <v>0.96789000000000003</v>
       </c>
     </row>
@@ -842,10 +841,10 @@
       <c r="C23">
         <v>10</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>4.9100000000000003E-3</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <v>0.96825000000000006</v>
       </c>
     </row>
@@ -859,10 +858,10 @@
       <c r="C24">
         <v>15</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <v>6.9899999999999997E-3</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <v>0.96826000000000001</v>
       </c>
     </row>
@@ -876,10 +875,10 @@
       <c r="C25">
         <v>20</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <v>9.7199999999999995E-3</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <v>0.96828999999999998</v>
       </c>
     </row>
@@ -893,11 +892,11 @@
       <c r="C26">
         <v>5</v>
       </c>
-      <c r="D26">
-        <v>7.9600000000000001E-3</v>
+      <c r="D26" s="2">
+        <v>7.9000000000000008E-3</v>
       </c>
       <c r="E26" s="2">
-        <v>0.87516000000000005</v>
+        <v>0.87485999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -910,11 +909,11 @@
       <c r="C27">
         <v>10</v>
       </c>
-      <c r="D27">
-        <v>1.0970000000000001E-2</v>
+      <c r="D27" s="3">
+        <v>1.081E-2</v>
       </c>
       <c r="E27" s="2">
-        <v>0.91579999999999995</v>
+        <v>0.91644999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -927,11 +926,11 @@
       <c r="C28">
         <v>15</v>
       </c>
-      <c r="D28">
-        <v>1.5010000000000001E-2</v>
+      <c r="D28" s="3">
+        <v>1.498E-2</v>
       </c>
       <c r="E28" s="2">
-        <v>0.92727999999999999</v>
+        <v>0.92728999999999995</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -944,11 +943,11 @@
       <c r="C29">
         <v>20</v>
       </c>
-      <c r="D29">
-        <v>2.1309999999999999E-2</v>
+      <c r="D29" s="3">
+        <v>2.1250000000000002E-2</v>
       </c>
       <c r="E29" s="2">
-        <v>0.93313999999999997</v>
+        <v>0.93308999999999997</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1029,10 +1028,10 @@
       <c r="C34">
         <v>5</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <v>3.5100000000000001E-3</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <v>0.91344999999999998</v>
       </c>
     </row>
@@ -1046,10 +1045,10 @@
       <c r="C35">
         <v>10</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2">
         <v>4.9800000000000001E-3</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <v>0.92979999999999996</v>
       </c>
     </row>
@@ -1063,10 +1062,10 @@
       <c r="C36">
         <v>15</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2">
         <v>6.79E-3</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <v>0.93398999999999999</v>
       </c>
     </row>
@@ -1080,10 +1079,10 @@
       <c r="C37">
         <v>20</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2">
         <v>8.8800000000000007E-3</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <v>0.93342999999999998</v>
       </c>
     </row>
@@ -1097,10 +1096,10 @@
       <c r="C38">
         <v>5</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2">
         <v>3.8999999999999999E-4</v>
       </c>
-      <c r="E38" s="3">
+      <c r="E38" s="2">
         <v>0.9214</v>
       </c>
     </row>
@@ -1114,10 +1113,10 @@
       <c r="C39">
         <v>10</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>8.4999999999999995E-4</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E39" s="2">
         <v>0.91573000000000004</v>
       </c>
     </row>
@@ -1131,10 +1130,10 @@
       <c r="C40">
         <v>15</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <v>1.2899999999999999E-3</v>
       </c>
-      <c r="E40" s="3">
+      <c r="E40" s="2">
         <v>0.91934000000000005</v>
       </c>
     </row>
@@ -1148,10 +1147,10 @@
       <c r="C41">
         <v>20</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2">
         <v>1.65E-3</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E41" s="2">
         <v>0.92434000000000005</v>
       </c>
     </row>
@@ -1165,10 +1164,10 @@
       <c r="C42">
         <v>5</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2">
         <v>1.6160000000000001E-2</v>
       </c>
-      <c r="E42" s="3">
+      <c r="E42" s="2">
         <v>0.94879000000000002</v>
       </c>
     </row>
@@ -1182,10 +1181,10 @@
       <c r="C43">
         <v>10</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2">
         <v>2.4740000000000002E-2</v>
       </c>
-      <c r="E43" s="3">
+      <c r="E43" s="2">
         <v>0.95355999999999996</v>
       </c>
     </row>
@@ -1199,10 +1198,10 @@
       <c r="C44">
         <v>15</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <v>3.3340000000000002E-2</v>
       </c>
-      <c r="E44" s="3">
+      <c r="E44" s="2">
         <v>0.95631999999999995</v>
       </c>
     </row>
@@ -1216,10 +1215,10 @@
       <c r="C45">
         <v>20</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2">
         <v>3.9269999999999999E-2</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E45" s="2">
         <v>0.95855000000000001</v>
       </c>
     </row>

</xml_diff>